<commit_message>
Currently working on Queue ADT
</commit_message>
<xml_diff>
--- a/DSA by Shradha Didi & Aman Bhaiya.xlsx
+++ b/DSA by Shradha Didi & Aman Bhaiya.xlsx
@@ -16,14 +16,14 @@
   </definedNames>
   <calcPr calcId="124519"/>
   <customWorkbookViews>
+    <customWorkbookView name="Filter 1" guid="{5451177E-605B-4368-AC7B-D46C41798C55}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
     <customWorkbookView name="Filter 2" guid="{C1A4E709-E9F1-4376-A047-F26FFC5F2C8F}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
-    <customWorkbookView name="Filter 1" guid="{5451177E-605B-4368-AC7B-D46C41798C55}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="898" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="899" uniqueCount="468">
   <si>
     <t>DSA by Shradha Didi &amp; Aman Bhaiya</t>
   </si>
@@ -1798,6 +1798,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1808,10 +1812,6 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2026,8 +2026,8 @@
   </sheetPr>
   <dimension ref="A1:Z919"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
@@ -2039,12 +2039,12 @@
     <col min="7" max="7" width="26.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:26" ht="32.25" customHeight="1">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
@@ -2070,11 +2070,11 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -2100,9 +2100,9 @@
       <c r="Z2" s="2"/>
     </row>
     <row r="3" spans="1:26" ht="15">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -2128,9 +2128,9 @@
       <c r="Z3" s="2"/>
     </row>
     <row r="4" spans="1:26" ht="15">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -2221,7 +2221,7 @@
       <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="42" t="s">
+      <c r="C7" s="44" t="s">
         <v>6</v>
       </c>
       <c r="D7" s="2"/>
@@ -2255,7 +2255,7 @@
       <c r="B8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="40"/>
+      <c r="C8" s="42"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -2382,7 +2382,7 @@
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="2"/>
-      <c r="E12" s="43" t="s">
+      <c r="E12" s="39" t="s">
         <v>467</v>
       </c>
       <c r="F12" s="2"/>
@@ -2416,7 +2416,7 @@
       </c>
       <c r="C13" s="12"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="39" t="s">
         <v>467</v>
       </c>
       <c r="F13" s="2"/>
@@ -3263,7 +3263,7 @@
       <c r="B39" s="19"/>
       <c r="C39" s="20"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="44"/>
+      <c r="E39" s="40"/>
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -3295,7 +3295,7 @@
       </c>
       <c r="C40" s="20"/>
       <c r="D40" s="2"/>
-      <c r="E40" s="43" t="s">
+      <c r="E40" s="39" t="s">
         <v>467</v>
       </c>
       <c r="F40" s="2"/>
@@ -3329,7 +3329,7 @@
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="2"/>
-      <c r="E41" s="43" t="s">
+      <c r="E41" s="39" t="s">
         <v>467</v>
       </c>
       <c r="F41" s="2"/>
@@ -3367,7 +3367,7 @@
       <c r="D42" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E42" s="43" t="s">
+      <c r="E42" s="39" t="s">
         <v>467</v>
       </c>
       <c r="F42" s="2"/>
@@ -3401,7 +3401,7 @@
       </c>
       <c r="C43" s="20"/>
       <c r="D43" s="2"/>
-      <c r="E43" s="43" t="s">
+      <c r="E43" s="39" t="s">
         <v>467</v>
       </c>
       <c r="F43" s="2"/>
@@ -3437,7 +3437,7 @@
         <v>57</v>
       </c>
       <c r="D44" s="2"/>
-      <c r="E44" s="43" t="s">
+      <c r="E44" s="39" t="s">
         <v>467</v>
       </c>
       <c r="F44" s="2"/>
@@ -3471,7 +3471,9 @@
       </c>
       <c r="C45" s="20"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="2"/>
+      <c r="E45" s="39" t="s">
+        <v>467</v>
+      </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
@@ -29182,13 +29184,13 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{5451177E-605B-4368-AC7B-D46C41798C55}" filter="1" showAutoFilter="1">
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A293:C332"/>
+    </customSheetView>
     <customSheetView guid="{C1A4E709-E9F1-4376-A047-F26FFC5F2C8F}" filter="1" showAutoFilter="1">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <autoFilter ref="A11:C37"/>
-    </customSheetView>
-    <customSheetView guid="{5451177E-605B-4368-AC7B-D46C41798C55}" filter="1" showAutoFilter="1">
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A293:C332"/>
     </customSheetView>
   </customSheetViews>
   <mergeCells count="3">
@@ -29597,28 +29599,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
     </row>
     <row r="2" spans="1:3" ht="12.75">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="40"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="3"/>

</xml_diff>